<commit_message>
recovered glider 327. added recovered ingest sheet and updated cal info with recovered date.
</commit_message>
<xml_diff>
--- a/CE05MOAS-GL327/Omaha_Cal_Info_CE05MOAS-GL327_00002.xlsx
+++ b/CE05MOAS-GL327/Omaha_Cal_Info_CE05MOAS-GL327_00002.xlsx
@@ -35,7 +35,7 @@
     <definedName name="_FilterDatabase_1_1_1">Moorings!$A$1:$J$78</definedName>
     <definedName name="_FilterDatabase_2">Asset_Cal_Info!$A$1:$F$276</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -750,7 +750,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -818,7 +818,9 @@
       <c r="E2" s="6">
         <v>0.7090277777777777</v>
       </c>
-      <c r="F2" s="7"/>
+      <c r="F2" s="7">
+        <v>42357</v>
+      </c>
       <c r="G2" s="8" t="s">
         <v>31</v>
       </c>
@@ -854,7 +856,7 @@
   <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>